<commit_message>
added schedule option for teachers - no error catching yet for classes which don't exist
</commit_message>
<xml_diff>
--- a/helper sql.xlsx
+++ b/helper sql.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\OneDrive\Brooklyn College\5-Bklyn College Fall 2020\MDY Database\MDY Attendance App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628B8DC6-2D66-46A6-AA49-B072071FF89E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B50E21-8521-49E4-9B9C-17604E77EA04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30810" yWindow="1635" windowWidth="21600" windowHeight="11385" xr2:uid="{188F6493-CB32-4A3F-81E1-A6A252778801}"/>
+    <workbookView xWindow="28680" yWindow="60" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{188F6493-CB32-4A3F-81E1-A6A252778801}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -495,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2064F20-83ED-4FA7-A432-D94AB296E061}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -546,7 +547,7 @@
         <v>32</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D17" si="0">B2</f>
+        <f t="shared" ref="D2:D16" si="0">B2</f>
         <v>7G-102'</v>
       </c>
       <c r="E2" t="s">
@@ -929,4 +930,16 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150CF83D-D203-497D-B5BD-C6B90E272E8B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
extended registration abilities to add subject and classes, added content-sections behind main content, redesigned headings, this commit is NOT complete but uploading it for testing purposes
</commit_message>
<xml_diff>
--- a/helper sql.xlsx
+++ b/helper sql.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\OneDrive\Brooklyn College\5-Bklyn College Fall 2020\MDY Database\MDY Attendance App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B50E21-8521-49E4-9B9C-17604E77EA04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59A7AF6-55A6-4FFE-983E-85BFED0B99CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="60" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{188F6493-CB32-4A3F-81E1-A6A252778801}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="58">
   <si>
     <t>7-101</t>
   </si>
@@ -137,6 +137,78 @@
   </si>
   <si>
     <t xml:space="preserve"> where classid like '</t>
+  </si>
+  <si>
+    <t>ELA</t>
+  </si>
+  <si>
+    <t>Jewish History</t>
+  </si>
+  <si>
+    <t>Nabi</t>
+  </si>
+  <si>
+    <t>Parasha</t>
+  </si>
+  <si>
+    <t>Social Studies</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>Halacha</t>
+  </si>
+  <si>
+    <t>Safe</t>
+  </si>
+  <si>
+    <t>Humash</t>
+  </si>
+  <si>
+    <t>Safah</t>
+  </si>
+  <si>
+    <t>Hashkafah</t>
+  </si>
+  <si>
+    <t>Keria</t>
+  </si>
+  <si>
+    <t>Gemara</t>
+  </si>
+  <si>
+    <t>Judaic Studies</t>
+  </si>
+  <si>
+    <t>Tamim</t>
+  </si>
+  <si>
+    <t>Judaic  Studies</t>
+  </si>
+  <si>
+    <t>Computers</t>
+  </si>
+  <si>
+    <t>JewishHistory</t>
+  </si>
+  <si>
+    <t>SocialStudies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">('ELA', 'ELA'), ('Computers', 'Computers'), ('Gemara', 'Gemara'), ('Halacha', 'Halacha'), ('Hashkafah', 'Hashkafah'), ('Humash', 'Humash'), ('JewishHistory', 'Jewish History'), ('Judaic Studies', 'Judaic  Studies'), ('Keria', 'Keria'), ('Math', 'Math'), ('Nabi', 'Nabi'), ('Parasha', 'Parasha'), ('Safah', 'Safah'), ('Safe', 'Safe'), ('Science', 'Science'), ('SocialStudies', 'Social Studies'), ('Tamim', 'Tamim'), </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'8G-101', '8G-102', '8G-103', '8G-111', '8B-201', '8B-202', '8B-203', '8B-211', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8G-103' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">('7-101', '7G-101'), ('7-102', '7G-102'), ('7-103', '7G-103'), ('7-111', '7G-111'), ('7-201', '7B-201'), ('7-202', '7B-202'), ('7-203', '7B-203'), ('7-211', '7B-211'), </t>
   </si>
 </sst>
 </file>
@@ -178,8 +250,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2064F20-83ED-4FA7-A432-D94AB296E061}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="C22" sqref="C22:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +578,7 @@
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -924,6 +997,205 @@
       <c r="H16" t="str">
         <f t="shared" si="2"/>
         <v>update course set classid3 = '8B-211'  where classid like '8-211%';</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" t="str">
+        <f>"'"&amp;B22&amp;", "</f>
+        <v xml:space="preserve">'7G-101', </v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" ref="D23:D37" si="3">"'"&amp;B23&amp;", "</f>
+        <v xml:space="preserve">'7G-102', </v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'7G-103', </v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'7G-111', </v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'7B-201', </v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'7B-202', </v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'7B-203', </v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'7B-211', </v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'8G-101', </v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'8G-102', </v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'8G-103', </v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'8G-111', </v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'8B-201', </v>
+      </c>
+      <c r="I34" t="str">
+        <f>_xlfn.CONCAT(D30:D37)</f>
+        <v xml:space="preserve">'8G-101', '8G-102', '8G-103', '8G-111', '8B-201', '8B-202', '8B-203', '8B-211', </v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'8B-202', </v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'8B-203', </v>
+      </c>
+      <c r="I36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">'8B-211', </v>
       </c>
     </row>
   </sheetData>
@@ -934,12 +1206,432 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150CF83D-D203-497D-B5BD-C6B90E272E8B}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"('"&amp;A2&amp;"', '"&amp;B2&amp;"'), "</f>
+        <v xml:space="preserve">('ELA', 'ELA'), </v>
+      </c>
+      <c r="E2" t="str">
+        <f>_xlfn.CONCAT(C2:C18)</f>
+        <v xml:space="preserve">('ELA', 'ELA'), ('Computers', 'Computers'), ('Gemara', 'Gemara'), ('Halacha', 'Halacha'), ('Hashkafah', 'Hashkafah'), ('Humash', 'Humash'), ('JewishHistory', 'Jewish History'), ('Judaic Studies', 'Judaic  Studies'), ('Keria', 'Keria'), ('Math', 'Math'), ('Nabi', 'Nabi'), ('Parasha', 'Parasha'), ('Safah', 'Safah'), ('Safe', 'Safe'), ('Science', 'Science'), ('SocialStudies', 'Social Studies'), ('Tamim', 'Tamim'), </v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C18" si="0">"('"&amp;A3&amp;"', '"&amp;B3&amp;"'), "</f>
+        <v xml:space="preserve">('Computers', 'Computers'), </v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Gemara', 'Gemara'), </v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Halacha', 'Halacha'), </v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Hashkafah', 'Hashkafah'), </v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Humash', 'Humash'), </v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('JewishHistory', 'Jewish History'), </v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Judaic Studies', 'Judaic  Studies'), </v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Keria', 'Keria'), </v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Math', 'Math'), </v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Nabi', 'Nabi'), </v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Parasha', 'Parasha'), </v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Safah', 'Safah'), </v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Safe', 'Safe'), </v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Science', 'Science'), </v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('SocialStudies', 'Social Studies'), </v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">('Tamim', 'Tamim'), </v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="str">
+        <f>"('"&amp;A22&amp;"', '"&amp;B22&amp;"), "</f>
+        <v xml:space="preserve">('7-101', '7G-101'), </v>
+      </c>
+      <c r="D22" t="str">
+        <f>_xlfn.CONCAT(C22:C29)</f>
+        <v xml:space="preserve">('7-101', '7G-101'), ('7-102', '7G-102'), ('7-103', '7G-103'), ('7-111', '7G-111'), ('7-201', '7B-201'), ('7-202', '7B-202'), ('7-203', '7B-203'), ('7-211', '7B-211'), </v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" ref="C23:C37" si="1">"('"&amp;A23&amp;"', '"&amp;B23&amp;"), "</f>
+        <v xml:space="preserve">('7-102', '7G-102'), </v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('7-103', '7G-103'), </v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('7-111', '7G-111'), </v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('7-201', '7B-201'), </v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('7-202', '7B-202'), </v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('7-203', '7B-203'), </v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('7-211', '7B-211'), </v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('8-101', '8G-101'), </v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('8-102', '8G-102'), </v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('8-103', '8G-103' ), </v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('8-111', '8G-111'), </v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('8-201', '8B-201'), </v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('8-202', '8B-202'), </v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('8-203', '8B-203'), </v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">('8-211', '8B-211'), </v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:B17">
+    <sortCondition ref="B12:B17"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added Friday to schedule
</commit_message>
<xml_diff>
--- a/helper sql.xlsx
+++ b/helper sql.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\OneDrive\Brooklyn College\5-Bklyn College Fall 2020\MDY Database\MDY Attendance App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59A7AF6-55A6-4FFE-983E-85BFED0B99CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4557D4-349D-4643-83C2-C9720FC8B3A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="60" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{188F6493-CB32-4A3F-81E1-A6A252778801}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="117">
   <si>
     <t>7-101</t>
   </si>
@@ -209,6 +209,183 @@
   </si>
   <si>
     <t xml:space="preserve">('7-101', '7G-101'), ('7-102', '7G-102'), ('7-103', '7G-103'), ('7-111', '7G-111'), ('7-201', '7B-201'), ('7-202', '7B-202'), ('7-203', '7B-203'), ('7-211', '7B-211'), </t>
+  </si>
+  <si>
+    <t>A_F1</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>0-0-0</t>
+  </si>
+  <si>
+    <t>rfriedman</t>
+  </si>
+  <si>
+    <t>scheduleid</t>
+  </si>
+  <si>
+    <t>periodid</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>courseid</t>
+  </si>
+  <si>
+    <t>sort</t>
+  </si>
+  <si>
+    <t>courseid2</t>
+  </si>
+  <si>
+    <t>classid2</t>
+  </si>
+  <si>
+    <t>teacher</t>
+  </si>
+  <si>
+    <t>A_F2</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>A_F3</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>A_F4</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>A_F5</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>A_F6</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>A_F7</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>B_F1</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>B_F2</t>
+  </si>
+  <si>
+    <t>B_F3</t>
+  </si>
+  <si>
+    <t>B_F4</t>
+  </si>
+  <si>
+    <t>B_F5</t>
+  </si>
+  <si>
+    <t>B_F6</t>
+  </si>
+  <si>
+    <t>B_F7</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('</t>
+  </si>
+  <si>
+    <t>A_FL</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>B_FL</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F1', 'F1', 'A', '0-0-0', '89', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F2', 'F2', 'A', '0-0-0', '90', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F3', 'F3', 'A', '0-0-0', '91', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F4', 'F4', 'A', '0-0-0', '92', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_FL', 'FL', 'A', '0-0-0', '93', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F5', 'F5', 'A', '0-0-0', '94', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F6', 'F6', 'A', '0-0-0', '95', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F7', 'F7', 'A', '0-0-0', '96', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F1', 'F1', 'B', '0-0-0', '97', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F2', 'F2', 'B', '0-0-0', '98', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F3', 'F3', 'B', '0-0-0', '99', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F4', 'F4', 'B', '0-0-0', '100', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_FL', 'FL', 'B', '0-0-0', '101', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F5', 'F5', 'B', '0-0-0', '102', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F6', 'F6', 'B', '0-0-0', '103', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F7', 'F7', 'B', '0-0-0', '104', 'rfriedman');</t>
+  </si>
+  <si>
+    <t>A_F2jsmith2</t>
+  </si>
+  <si>
+    <t>7-101-Physics</t>
+  </si>
+  <si>
+    <t>7G-101-Physics</t>
+  </si>
+  <si>
+    <t>7G-101</t>
+  </si>
+  <si>
+    <t>jsmith2</t>
   </si>
 </sst>
 </file>
@@ -1206,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150CF83D-D203-497D-B5BD-C6B90E272E8B}">
-  <dimension ref="A2:E37"/>
+  <dimension ref="A2:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,7 +1745,7 @@
         <v xml:space="preserve">('8-103', '8G-103' ), </v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -1580,7 +1757,7 @@
         <v xml:space="preserve">('8-111', '8G-111'), </v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1592,7 +1769,7 @@
         <v xml:space="preserve">('8-201', '8B-201'), </v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1604,7 +1781,7 @@
         <v xml:space="preserve">('8-202', '8B-202'), </v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1616,7 +1793,7 @@
         <v xml:space="preserve">('8-203', '8B-203'), </v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -1626,12 +1803,551 @@
       <c r="C37" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">('8-211', '8B-211'), </v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" t="s">
+        <v>68</v>
+      </c>
+      <c r="G40" t="s">
+        <v>69</v>
+      </c>
+      <c r="H40" t="s">
+        <v>70</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41">
+        <v>89</v>
+      </c>
+      <c r="H41" t="s">
+        <v>62</v>
+      </c>
+      <c r="J41" t="s">
+        <v>92</v>
+      </c>
+      <c r="K41" t="str">
+        <f>J41&amp;A41&amp;"', '"&amp;B41 &amp;"', '"&amp;C41&amp;"', '"&amp;D41&amp;"', '"&amp;E41&amp;"', '"&amp;H41&amp;"');"</f>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F1', 'F1', 'A', '0-0-0', '89', 'rfriedman');</v>
+      </c>
+      <c r="L41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42">
+        <v>90</v>
+      </c>
+      <c r="H42" t="s">
+        <v>62</v>
+      </c>
+      <c r="J42" t="s">
+        <v>92</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" ref="K42:K56" si="2">J42&amp;A42&amp;"', '"&amp;B42 &amp;"', '"&amp;C42&amp;"', '"&amp;D42&amp;"', '"&amp;E42&amp;"', '"&amp;H42&amp;"');"</f>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F2', 'F2', 'A', '0-0-0', '90', 'rfriedman');</v>
+      </c>
+      <c r="L42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43">
+        <v>91</v>
+      </c>
+      <c r="H43" t="s">
+        <v>62</v>
+      </c>
+      <c r="J43" t="s">
+        <v>92</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F3', 'F3', 'A', '0-0-0', '91', 'rfriedman');</v>
+      </c>
+      <c r="L43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44">
+        <v>92</v>
+      </c>
+      <c r="H44" t="s">
+        <v>62</v>
+      </c>
+      <c r="J44" t="s">
+        <v>92</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F4', 'F4', 'A', '0-0-0', '92', 'rfriedman');</v>
+      </c>
+      <c r="L44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45">
+        <v>93</v>
+      </c>
+      <c r="H45" t="s">
+        <v>62</v>
+      </c>
+      <c r="J45" t="s">
+        <v>92</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_FL', 'FL', 'A', '0-0-0', '93', 'rfriedman');</v>
+      </c>
+      <c r="L45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46">
+        <v>94</v>
+      </c>
+      <c r="H46" t="s">
+        <v>62</v>
+      </c>
+      <c r="J46" t="s">
+        <v>92</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F5', 'F5', 'A', '0-0-0', '94', 'rfriedman');</v>
+      </c>
+      <c r="L46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" t="s">
+        <v>61</v>
+      </c>
+      <c r="E47">
+        <v>95</v>
+      </c>
+      <c r="H47" t="s">
+        <v>62</v>
+      </c>
+      <c r="J47" t="s">
+        <v>92</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F6', 'F6', 'A', '0-0-0', '95', 'rfriedman');</v>
+      </c>
+      <c r="L47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" t="s">
+        <v>61</v>
+      </c>
+      <c r="E48">
+        <v>96</v>
+      </c>
+      <c r="H48" t="s">
+        <v>62</v>
+      </c>
+      <c r="J48" t="s">
+        <v>92</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('A_F7', 'F7', 'A', '0-0-0', '96', 'rfriedman');</v>
+      </c>
+      <c r="L48" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" t="s">
+        <v>61</v>
+      </c>
+      <c r="E49">
+        <v>97</v>
+      </c>
+      <c r="H49" t="s">
+        <v>62</v>
+      </c>
+      <c r="J49" t="s">
+        <v>92</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F1', 'F1', 'B', '0-0-0', '97', 'rfriedman');</v>
+      </c>
+      <c r="L49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" t="s">
+        <v>61</v>
+      </c>
+      <c r="E50">
+        <v>98</v>
+      </c>
+      <c r="H50" t="s">
+        <v>62</v>
+      </c>
+      <c r="J50" t="s">
+        <v>92</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F2', 'F2', 'B', '0-0-0', '98', 'rfriedman');</v>
+      </c>
+      <c r="L50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51">
+        <v>99</v>
+      </c>
+      <c r="H51" t="s">
+        <v>62</v>
+      </c>
+      <c r="J51" t="s">
+        <v>92</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F3', 'F3', 'B', '0-0-0', '99', 'rfriedman');</v>
+      </c>
+      <c r="L51" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" t="s">
+        <v>61</v>
+      </c>
+      <c r="E52">
+        <v>100</v>
+      </c>
+      <c r="H52" t="s">
+        <v>62</v>
+      </c>
+      <c r="J52" t="s">
+        <v>92</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F4', 'F4', 'B', '0-0-0', '100', 'rfriedman');</v>
+      </c>
+      <c r="L52" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>95</v>
+      </c>
+      <c r="B53" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53">
+        <v>101</v>
+      </c>
+      <c r="H53" t="s">
+        <v>62</v>
+      </c>
+      <c r="J53" t="s">
+        <v>92</v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_FL', 'FL', 'B', '0-0-0', '101', 'rfriedman');</v>
+      </c>
+      <c r="L53" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" t="s">
+        <v>61</v>
+      </c>
+      <c r="E54">
+        <v>102</v>
+      </c>
+      <c r="H54" t="s">
+        <v>62</v>
+      </c>
+      <c r="J54" t="s">
+        <v>92</v>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F5', 'F5', 'B', '0-0-0', '102', 'rfriedman');</v>
+      </c>
+      <c r="L54" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>89</v>
+      </c>
+      <c r="B55" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" t="s">
+        <v>61</v>
+      </c>
+      <c r="E55">
+        <v>103</v>
+      </c>
+      <c r="H55" t="s">
+        <v>62</v>
+      </c>
+      <c r="J55" t="s">
+        <v>92</v>
+      </c>
+      <c r="K55" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F6', 'F6', 'B', '0-0-0', '103', 'rfriedman');</v>
+      </c>
+      <c r="L55" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" t="s">
+        <v>61</v>
+      </c>
+      <c r="E56">
+        <v>104</v>
+      </c>
+      <c r="H56" t="s">
+        <v>62</v>
+      </c>
+      <c r="J56" t="s">
+        <v>92</v>
+      </c>
+      <c r="K56" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into schedule (scheduleid, periodid, week, courseid, sort, teacher) values ('B_F7', 'F7', 'B', '0-0-0', '104', 'rfriedman');</v>
+      </c>
+      <c r="L56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" t="s">
+        <v>72</v>
+      </c>
+      <c r="D62" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" t="s">
+        <v>113</v>
+      </c>
+      <c r="F62">
+        <v>29</v>
+      </c>
+      <c r="G62" t="s">
+        <v>114</v>
+      </c>
+      <c r="H62" t="s">
+        <v>115</v>
+      </c>
+      <c r="I62" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:B17">
     <sortCondition ref="B12:B17"/>
   </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>